<commit_message>
new data from Ed
</commit_message>
<xml_diff>
--- a/data/PVT Data For Marcelo.xlsx
+++ b/data/PVT Data For Marcelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjdaqua\Python\Projects\HGOR\Code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044AA981-18AC-4AF9-A79E-D3EBB848A292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9018B93-11C9-488B-B6BE-A1145F771076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$I$2:$Q$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$2:$Q$178</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1598,13 +1598,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1691,7 +1692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1899,7 +1900,7 @@
         <v>5.5599417318106506E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -2001,7 +2002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -2054,7 +2055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -2105,7 +2106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -2156,7 +2157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2258,7 +2259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -2309,7 +2310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -2360,7 +2361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -2411,7 +2412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -2513,7 +2514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
@@ -2564,7 +2565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
@@ -2615,7 +2616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
@@ -2666,7 +2667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
@@ -2717,7 +2718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
@@ -2768,7 +2769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -2872,7 +2873,7 @@
         <v>6.207016411351391E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
@@ -2977,7 +2978,7 @@
         <v>6.2735650788273449E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>15</v>
       </c>
@@ -3028,7 +3029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>15</v>
       </c>
@@ -3079,7 +3080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>15</v>
       </c>
@@ -3130,7 +3131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>15</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
@@ -3232,7 +3233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>15</v>
       </c>
@@ -3283,7 +3284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>15</v>
       </c>
@@ -3334,7 +3335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>15</v>
       </c>
@@ -3385,7 +3386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>15</v>
       </c>
@@ -3436,7 +3437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>15</v>
       </c>
@@ -3487,7 +3488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>15</v>
       </c>
@@ -3538,7 +3539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>15</v>
       </c>
@@ -3589,7 +3590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>15</v>
       </c>
@@ -3640,7 +3641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>15</v>
       </c>
@@ -3691,7 +3692,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>15</v>
       </c>
@@ -3793,7 +3794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>15</v>
       </c>
@@ -3844,7 +3845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>15</v>
       </c>
@@ -3895,7 +3896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>15</v>
       </c>
@@ -3999,7 +4000,7 @@
         <v>5.7769407632494139E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>15</v>
       </c>
@@ -4050,7 +4051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>15</v>
       </c>
@@ -4101,7 +4102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>15</v>
       </c>
@@ -4205,7 +4206,7 @@
         <v>5.6165260662974735E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>15</v>
       </c>
@@ -4256,7 +4257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>15</v>
       </c>
@@ -4360,7 +4361,7 @@
         <v>5.5389080596651176E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>15</v>
       </c>
@@ -4411,7 +4412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>15</v>
       </c>
@@ -4883,7 +4884,7 @@
         <v>5.4414957583540568E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>15</v>
       </c>
@@ -4936,7 +4937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>15</v>
       </c>
@@ -4987,7 +4988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>15</v>
       </c>
@@ -5038,7 +5039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>15</v>
       </c>
@@ -5089,7 +5090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>15</v>
       </c>
@@ -5140,7 +5141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>15</v>
       </c>
@@ -5191,7 +5192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>15</v>
       </c>
@@ -5242,7 +5243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>15</v>
       </c>
@@ -5452,7 +5453,7 @@
         <v>5.8540811726895403E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>15</v>
       </c>
@@ -5503,7 +5504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>15</v>
       </c>
@@ -5554,7 +5555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>15</v>
       </c>
@@ -5658,7 +5659,7 @@
         <v>5.9466466859338027E-4</v>
       </c>
     </row>
-    <row r="80" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>15</v>
       </c>
@@ -5917,7 +5918,7 @@
         <v>5.521140446770685E-4</v>
       </c>
     </row>
-    <row r="85" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>15</v>
       </c>
@@ -5968,7 +5969,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>15</v>
       </c>
@@ -6019,7 +6020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>15</v>
       </c>
@@ -6226,7 +6227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>15</v>
       </c>
@@ -6277,7 +6278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>15</v>
       </c>
@@ -6328,7 +6329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>15</v>
       </c>
@@ -6379,7 +6380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>15</v>
       </c>
@@ -6430,7 +6431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>15</v>
       </c>
@@ -6481,7 +6482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>15</v>
       </c>
@@ -6532,7 +6533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>15</v>
       </c>
@@ -6583,7 +6584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>15</v>
       </c>
@@ -6634,7 +6635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>15</v>
       </c>
@@ -6791,7 +6792,7 @@
         <v>6.0341290338152595E-4</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>15</v>
       </c>
@@ -6842,7 +6843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>15</v>
       </c>
@@ -6893,7 +6894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>15</v>
       </c>
@@ -6944,7 +6945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
         <v>15</v>
       </c>
@@ -7089,7 +7090,7 @@
       </c>
       <c r="Q107" s="13"/>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>15</v>
       </c>
@@ -7183,7 +7184,7 @@
       </c>
       <c r="Q109" s="13"/>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>15</v>
       </c>
@@ -7230,7 +7231,7 @@
       </c>
       <c r="Q110" s="13"/>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>15</v>
       </c>
@@ -7277,7 +7278,7 @@
       </c>
       <c r="Q111" s="13"/>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>15</v>
       </c>
@@ -7369,7 +7370,7 @@
       <c r="P113" s="18"/>
       <c r="Q113" s="13"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>15</v>
       </c>
@@ -7416,7 +7417,7 @@
       </c>
       <c r="Q114" s="13"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>15</v>
       </c>
@@ -7463,7 +7464,7 @@
       </c>
       <c r="Q115" s="13"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>15</v>
       </c>
@@ -7510,7 +7511,7 @@
       </c>
       <c r="Q116" s="13"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
         <v>15</v>
       </c>
@@ -7557,7 +7558,7 @@
       </c>
       <c r="Q117" s="13"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>15</v>
       </c>
@@ -7604,7 +7605,7 @@
       </c>
       <c r="Q118" s="13"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>15</v>
       </c>
@@ -7698,7 +7699,7 @@
       </c>
       <c r="Q120" s="13"/>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
         <v>15</v>
       </c>
@@ -7839,7 +7840,7 @@
       </c>
       <c r="Q123" s="13"/>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
         <v>15</v>
       </c>
@@ -7886,7 +7887,7 @@
       </c>
       <c r="Q124" s="13"/>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>14</v>
       </c>
@@ -7937,7 +7938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>14</v>
       </c>
@@ -7988,7 +7989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>14</v>
       </c>
@@ -8039,7 +8040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>14</v>
       </c>
@@ -8090,7 +8091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>14</v>
       </c>
@@ -8141,7 +8142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>14</v>
       </c>
@@ -8192,7 +8193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>14</v>
       </c>
@@ -8243,7 +8244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>14</v>
       </c>
@@ -8294,7 +8295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>14</v>
       </c>
@@ -8345,7 +8346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>14</v>
       </c>
@@ -8396,7 +8397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>14</v>
       </c>
@@ -8447,7 +8448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>14</v>
       </c>
@@ -8498,7 +8499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>14</v>
       </c>
@@ -8549,7 +8550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>14</v>
       </c>
@@ -8600,7 +8601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>14</v>
       </c>
@@ -8651,7 +8652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>14</v>
       </c>
@@ -8702,7 +8703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>14</v>
       </c>
@@ -8754,7 +8755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>14</v>
       </c>
@@ -8805,7 +8806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>14</v>
       </c>
@@ -8856,7 +8857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>14</v>
       </c>
@@ -8907,7 +8908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>14</v>
       </c>
@@ -8958,7 +8959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
         <v>14</v>
       </c>
@@ -9009,7 +9010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
         <v>14</v>
       </c>
@@ -9060,7 +9061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
         <v>14</v>
       </c>
@@ -9112,7 +9113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>14</v>
       </c>
@@ -9163,7 +9164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
         <v>14</v>
       </c>
@@ -9214,7 +9215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
         <v>14</v>
       </c>
@@ -9265,7 +9266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
         <v>14</v>
       </c>
@@ -9316,7 +9317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
         <v>14</v>
       </c>
@@ -9367,7 +9368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
         <v>14</v>
       </c>
@@ -9418,7 +9419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
         <v>14</v>
       </c>
@@ -9469,7 +9470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
         <v>14</v>
       </c>
@@ -9520,7 +9521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
         <v>14</v>
       </c>
@@ -9571,7 +9572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>14</v>
       </c>
@@ -9622,7 +9623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
         <v>14</v>
       </c>
@@ -9673,7 +9674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
         <v>14</v>
       </c>
@@ -9724,7 +9725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
         <v>14</v>
       </c>
@@ -9775,7 +9776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
         <v>14</v>
       </c>
@@ -9826,7 +9827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
         <v>14</v>
       </c>
@@ -9877,7 +9878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
         <v>14</v>
       </c>
@@ -9928,7 +9929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
         <v>13</v>
       </c>
@@ -9979,7 +9980,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
         <v>13</v>
       </c>
@@ -10030,7 +10031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
         <v>13</v>
       </c>
@@ -10081,7 +10082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
         <v>13</v>
       </c>
@@ -10132,7 +10133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
         <v>13</v>
       </c>
@@ -10183,7 +10184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
         <v>13</v>
       </c>
@@ -10234,7 +10235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
         <v>13</v>
       </c>
@@ -10285,7 +10286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
         <v>13</v>
       </c>
@@ -10336,7 +10337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
         <v>13</v>
       </c>
@@ -10387,7 +10388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
         <v>13</v>
       </c>
@@ -10438,7 +10439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
         <v>13</v>
       </c>
@@ -10489,7 +10490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
         <v>13</v>
       </c>
@@ -10540,7 +10541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
         <v>13</v>
       </c>
@@ -10591,7 +10592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="s">
         <v>13</v>
       </c>
@@ -10643,7 +10644,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C2:Q105" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:Q178" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="greaterThan" val="3000"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>